<commit_message>
2023-11-12 01:31:45 - download issue fixed
</commit_message>
<xml_diff>
--- a/server/output/output.xlsx
+++ b/server/output/output.xlsx
@@ -461,22 +461,22 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>Job</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Phones</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Emails</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -617,11 +617,7 @@
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>aidan.mccarron@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -684,11 +680,7 @@
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>john.higgins@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -810,11 +802,7 @@
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>michael.yohanis@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -936,11 +924,7 @@
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>declan.mc@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -1068,7 +1052,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>lorcan.mulvey@mcaleer-rushe.co.uk</t>
+          <t>lorcan.mulvey@mcaleer-rushe.co.uk , lorcanmulvey@yahoo.ie , lorcan.mulvey@yahoo.ie , lorcan.mulvey@berkeleygroup.co.uk</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1208,11 +1192,7 @@
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>gerald.laverty@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
@@ -1472,11 +1452,7 @@
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>steve.morris@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
@@ -1604,7 +1580,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>lee.gray@mcaleer-rushe.co.uk</t>
+          <t>leergray3@hotmail.co.uk , lee.gray@mcaleer-rushe.co.uk</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1744,11 +1720,7 @@
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>eamonn.laverty@thorntonroofing.com</t>
-        </is>
-      </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -1861,11 +1833,7 @@
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>eoin.gormley@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
@@ -1987,11 +1955,7 @@
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>paddy.connolly@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
@@ -2113,11 +2077,7 @@
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>daisy.butterworth@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
@@ -2239,11 +2199,7 @@
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>sinead.gorman@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
@@ -2371,7 +2327,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>connor.graham@mcaleer-rushe.co.uk</t>
+          <t>connor.graham@patton.co.uk , connor.graham@mcaleer-rushe.co.uk</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -2509,7 +2465,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>cathal.magee@mcaleer-rushe.co.uk</t>
+          <t>cathal.magee@mcaleer-rushe.co.uk , cathal.magee1@hotmail.co.uk</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -2787,11 +2743,7 @@
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>nina.salandy@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
@@ -2913,11 +2865,7 @@
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>peter.coyle@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
@@ -3039,11 +2987,7 @@
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>orran.devine@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
@@ -3165,11 +3109,7 @@
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>niamh.heneghan@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>

</xml_diff>

<commit_message>
2023-11-12 02:46:14 - fixed github
</commit_message>
<xml_diff>
--- a/server/output/output.xlsx
+++ b/server/output/output.xlsx
@@ -456,22 +456,22 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>Job</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Phones</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Emails</t>
         </is>
       </c>
     </row>
@@ -507,11 +507,7 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>aidan.mccarron@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -526,7 +522,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Higgins</t>
+          <t>Higgins MCIOB</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -545,11 +541,7 @@
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>john.higgins@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -564,7 +556,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Yohanis</t>
+          <t>Yohanis MCIOB</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -583,11 +575,7 @@
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>michael.yohanis@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -602,7 +590,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Mc</t>
+          <t>McLogan CMIOSH LL.M</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -621,11 +609,7 @@
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>declan.mc@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -665,7 +649,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>lorcan.mulvey@mcaleer-rushe.co.uk</t>
+          <t>lorcan.mulvey@mcaleer-rushe.co.uk , lorcanmulvey@yahoo.ie , lorcan.mulvey@yahoo.ie , lorcan.mulvey@berkeleygroup.co.uk</t>
         </is>
       </c>
     </row>
@@ -701,11 +685,7 @@
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>gerald.laverty@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -781,11 +761,7 @@
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>steve.morris@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -800,7 +776,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Gray Grad</t>
+          <t>Gray GradIOSH</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -825,7 +801,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>lee.gray@mcaleer-rushe.co.uk</t>
+          <t>leergray3@hotmail.co.uk , lee.gray@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -842,7 +818,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Laverty</t>
+          <t>Laverty. MCIOB</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -861,11 +837,7 @@
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>eamonn.laverty@thorntonroofing.com</t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -899,11 +871,7 @@
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>eoin.gormley@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -937,11 +905,7 @@
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>paddy.connolly@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -975,11 +939,7 @@
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>daisy.butterworth@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -994,7 +954,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Gorman</t>
+          <t>Gorman (she/her)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1013,11 +973,7 @@
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>sinead.gorman@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1057,7 +1013,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>connor.graham@mcaleer-rushe.co.uk</t>
+          <t>connor.graham@patton.co.uk , connor.graham@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -1099,7 +1055,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>cathal.magee@mcaleer-rushe.co.uk</t>
+          <t>cathal.magee@mcaleer-rushe.co.uk , cathal.magee1@hotmail.co.uk</t>
         </is>
       </c>
     </row>
@@ -1158,7 +1114,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Salandy</t>
+          <t>Salandy    BSc. (Hons.) GradIOSH</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1177,11 +1133,7 @@
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>nina.salandy@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1215,11 +1167,7 @@
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>peter.coyle@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1253,11 +1201,7 @@
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>orran.devine@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1291,11 +1235,7 @@
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>niamh.heneghan@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
2023-11-14 16:04:08 - name corrections
</commit_message>
<xml_diff>
--- a/server/output/output.xlsx
+++ b/server/output/output.xlsx
@@ -456,29 +456,29 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Job</t>
+          <t>Title</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Country</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Phones</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Emails</t>
+          <t>Email</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Aidan Mc</t>
+          <t>Aidan McCarron</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mccarron</t>
+          <t>McCarron</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -507,12 +507,16 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>aidan.mccarron@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>John Higgins</t>
+          <t xml:space="preserve">John Higgins </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -522,7 +526,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Higgins MCIOB</t>
+          <t>Higgins</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -541,12 +545,16 @@
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>john.higgins@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Michael Yohanis</t>
+          <t xml:space="preserve">Michael Yohanis </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -556,7 +564,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Yohanis MCIOB</t>
+          <t>Yohanis</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -575,12 +583,16 @@
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>michael.yohanis@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Declan Mc</t>
+          <t>Declan McLogan</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -590,7 +602,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>McLogan CMIOSH LL.M</t>
+          <t>McLogan</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -609,7 +621,11 @@
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>declan.mclogan@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -649,7 +665,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>lorcan.mulvey@mcaleer-rushe.co.uk , lorcanmulvey@yahoo.ie , lorcan.mulvey@yahoo.ie , lorcan.mulvey@berkeleygroup.co.uk</t>
+          <t>lorcan.mulvey@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -685,7 +701,11 @@
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>gerald.laverty@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -761,22 +781,26 @@
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>steve.morris@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Lee Robert Gray Grad</t>
+          <t xml:space="preserve">Lee Robert Gray </t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lee Robert</t>
+          <t>Lee</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Gray GradIOSH</t>
+          <t>Gray</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -801,7 +825,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>leergray3@hotmail.co.uk , lee.gray@mcaleer-rushe.co.uk</t>
+          <t>lee.gray@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -818,7 +842,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Laverty. MCIOB</t>
+          <t>Laverty</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -837,7 +861,11 @@
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>eamonn.laverty@thorntonroofing.com</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -871,7 +899,11 @@
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>eoin.gormley@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -905,7 +937,11 @@
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>paddy.connolly@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -939,7 +975,11 @@
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>daisy.butterworth@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -954,7 +994,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Gorman (she/her)</t>
+          <t>Gorman</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -973,7 +1013,11 @@
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>sinead.gorman@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1013,7 +1057,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>connor.graham@patton.co.uk , connor.graham@mcaleer-rushe.co.uk</t>
+          <t>connor.graham@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -1055,7 +1099,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>cathal.magee@mcaleer-rushe.co.uk , cathal.magee1@hotmail.co.uk</t>
+          <t>cathal.magee@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -1104,7 +1148,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Nina Salandy</t>
+          <t xml:space="preserve">Nina Salandy </t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1114,7 +1158,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Salandy    BSc. (Hons.) GradIOSH</t>
+          <t>Salandy</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1133,7 +1177,11 @@
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>nina.salandy@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1167,7 +1215,11 @@
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>peter.coyle@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1201,7 +1253,11 @@
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>orran.devine@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1235,7 +1291,11 @@
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>niamh.heneghan@mcaleer-rushe.co.uk</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
2023-11-15 02:56:12 - update the file
</commit_message>
<xml_diff>
--- a/server/output/output.xlsx
+++ b/server/output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,27 +451,32 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Linkedin</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Company</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
+          <t>Job</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Phones</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Emails</t>
         </is>
       </c>
     </row>
@@ -493,25 +498,26 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/aidan-mccarron-92416356</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>Project Director</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>aidan.mccarron@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -531,25 +537,26 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/john-higgins-mciob-b25b37a3</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Project Director</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Cookstown, Northern Ireland, United Kingdom</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>john.higgins@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -569,25 +576,26 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/michael-yohanis-mciob-060b5147</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>Project Director</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Belfast</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>michael.yohanis@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -607,25 +615,26 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/declan-mclogan-cmiosh-ll-m-48482613</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>Director of SHEQ</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Cookstown</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>declan.mclogan@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -645,27 +654,32 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/lorcan-mulvey-37ba7541</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>Project Director</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>London, England, United Kingdom</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>+44 7826 532410</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>lorcan.mulvey@mcaleer-rushe.co.uk</t>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>lorcan.mulvey@mcaleer-rushe.co.uk , lorcanmulvey@yahoo.ie , lorcan.mulvey@yahoo.ie , lorcan.mulvey@berkeleygroup.co.uk</t>
         </is>
       </c>
     </row>
@@ -687,25 +701,26 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/gerald-laverty-55a70790</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>Project Manager</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>London, England, United Kingdom</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>gerald.laverty@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -725,25 +740,30 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/darragh-greenan-5a2089b6</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>Contracts Director</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>London, United Kingdom</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>+44 7912 046630</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>darragh.greenan@mcaleer-rushe.co.uk</t>
         </is>
@@ -767,25 +787,26 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/steve-morris-05a32933</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>Project Director</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>Belfast Metropolitan Area</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>steve.morris@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -805,27 +826,32 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/lee-robert-gray-gradiosh-55b31a47</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>Senior SHEQ Advisor</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Newcastle upon Tyne, England, United Kingdom</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>07872331053</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>lee.gray@mcaleer-rushe.co.uk</t>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>leergray3@hotmail.co.uk , lee.gray@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -847,25 +873,26 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>https://linkedin.com/in/eamonn-laverty-mciob-9634b9b1</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>Thornton Roofing</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Construction Operations Manager</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>eamonn.laverty@thorntonroofing.com</t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -885,25 +912,26 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/eoin-gormley-10694a121</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>Project Director</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>London Area, United Kingdom</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>eoin.gormley@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -923,25 +951,26 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/paddy-connolly-3a4527102</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>Project Manager</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>Belfast, Northern Ireland, United Kingdom</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>paddy.connolly@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -961,25 +990,26 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/daisy-butterworth-14b437173</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>Assistant Project Manager</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>London, England, United Kingdom</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>daisy.butterworth@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -999,25 +1029,26 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/sinéad-gorman-she-her-523b9a64</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
           <t>SHEQ Officer</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>Belfast, United Kingdom</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>sinead.gorman@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1037,27 +1068,32 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/connor-graham-50b2b241</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>Head of Buying</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>Cookstown, N.Ireland</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>+44 28 2565 0003</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>connor.graham@mcaleer-rushe.co.uk</t>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>connor.graham@patton.co.uk , connor.graham@mcaleer-rushe.co.uk</t>
         </is>
       </c>
     </row>
@@ -1079,27 +1115,32 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/cathal-magee-a397ba8a</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>Health and Safety Officer</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>London, United Kingdom</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>+44 7835 631685</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>cathal.magee@mcaleer-rushe.co.uk</t>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>cathal.magee@mcaleer-rushe.co.uk , cathal.magee1@hotmail.co.uk</t>
         </is>
       </c>
     </row>
@@ -1121,25 +1162,30 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/bruno-antoniazzi</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>M&amp;E</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>Cookstown</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>+55 21 98139-3298 , +55 92 98855-0059 , +55 92 98802-4114</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>bruno.antoniazzi@mcaleer-rushe.co.uk</t>
         </is>
@@ -1163,25 +1209,26 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/nina-salandy-bsc-hons-gradiosh-4675955a</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
           <t>Snr. SHEQ Advisor</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>London, England, United Kingdom</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>nina.salandy@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1201,25 +1248,26 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/peter-coyle-854a8063</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>Senior Construction Manager</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>Belfast, United Kingdom</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>peter.coyle@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1239,25 +1287,26 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/orran-devine-b2715b166</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
           <t>Project Manager</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>Cookstown, Northern Ireland, United Kingdom</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>orran.devine@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1277,25 +1326,26 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>https://linkedin.com/in/niamh-heneghan-a98527197</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
+          <t>McAleer &amp; Rushe</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
           <t>Health and safety administrator</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>Wembley, England, United Kingdom</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>niamh.heneghan@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
2023-11-21 02:45:31 - location and phone nmubers added
</commit_message>
<xml_diff>
--- a/server/output/output.xlsx
+++ b/server/output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,76 +483,84 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Aidan McCarron</t>
+          <t>Paul Newman</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Aidan</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>McCarron</t>
+          <t>Newman</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/aidan-mccarron-92416356</t>
+          <t>https://linkedin.com/in/paul-newman-00a9a830</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Bow Transit Connectors</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Project Director</t>
+          <t>Construction Manager</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+          <t>Calgary, Alberta, Canada</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>+1 403-701-8000 , +1 403-589-9088 , +1 403-620-7239 , +1 410-340-7346 , +1 418-868-2428 , +1 403-640-3521</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>paul.newman@snclavalin.com , paul@pave-it.com , pnewman@bellsouth.net</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">John Higgins </t>
+          <t>Neil Lynchehaun</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Neil</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Higgins</t>
+          <t>Lynchehaun</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/john-higgins-mciob-b25b37a3</t>
+          <t>https://linkedin.com/in/neil-lynchehaun-23031ba4</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Project Director</t>
+          <t>Vice President, Special Projects</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Cookstown, Northern Ireland, United Kingdom</t>
+          <t>Calgary, Alberta, Canada</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -561,76 +569,84 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Michael Yohanis </t>
+          <t>Ken Tanner</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Ken</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Yohanis</t>
+          <t>Tanner</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/michael-yohanis-mciob-060b5147</t>
+          <t>https://linkedin.com/in/ken-tanner-9899939</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Project Director</t>
+          <t>Vice President Operations</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Belfast</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>+1 604-798-8491</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>ktanner@flatironcorp.com</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Declan McLogan</t>
+          <t>Octavio Flores</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Declan</t>
+          <t>Octavio</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>McLogan</t>
+          <t>Flores</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/declan-mclogan-cmiosh-ll-m-48482613</t>
+          <t>https://linkedin.com/in/octavio-flores-37b566a7</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Director of SHEQ</t>
+          <t>Area Operations Manager</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Cookstown</t>
+          <t>British Columbia, Canada</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -639,170 +655,178 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lorcan Mulvey</t>
+          <t>Jarred Gumbleton</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lorcan</t>
+          <t>Jarred</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Mulvey</t>
+          <t>Gumbleton</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/lorcan-mulvey-37ba7541</t>
+          <t>https://linkedin.com/in/jarredgumbleton</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Project Director</t>
+          <t>Project Manager</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>London, England, United Kingdom</t>
+          <t>Richmond, BC, Canada</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>+44 7826 532410</t>
+          <t>+1 250-272-6645</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>lorcan.mulvey@mcaleer-rushe.co.uk , lorcanmulvey@yahoo.ie , lorcan.mulvey@yahoo.ie , lorcan.mulvey@berkeleygroup.co.uk</t>
+          <t>jgumbleton@flatironcorp.com</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Gerald Laverty</t>
+          <t>Alicia Lopez</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Gerald</t>
+          <t>Alicia</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Laverty</t>
+          <t>Lopez</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/gerald-laverty-55a70790</t>
+          <t>https://linkedin.com/in/alicialopezcrespo</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>VP, Innovation &amp; Design</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>London, England, United Kingdom</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+          <t xml:space="preserve">USA and Canada </t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>DNC , DNC , +1 719-994-0855 , +1 720-232-3886 , DNC</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>acrespo@flatironcorp.com</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Darragh Greenan</t>
+          <t>Mike M</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Darragh</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Greenan</t>
+          <t>M</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/darragh-greenan-5a2089b6</t>
+          <t>https://linkedin.com/in/mike-meacher-031ba619</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Contracts Director</t>
+          <t>Quality Manager</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>London, United Kingdom</t>
+          <t>British Columbia, Canada</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>+44 7912 046630</t>
+          <t>+1 604-363-4558</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>darragh.greenan@mcaleer-rushe.co.uk</t>
+          <t>mike.meacher@lafarge-na.com , mmeacher@fwsgroup.com , mmeacher@flatironcorp.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Steve Morris</t>
+          <t>Donald Dow</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Steve</t>
+          <t>Donald</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Morris</t>
+          <t>Dow</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/steve-morris-05a32933</t>
+          <t>https://linkedin.com/in/donald-dow-7518ab192</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>AFDE Partnership</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Project Director</t>
+          <t>Safety Manager</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Belfast Metropolitan Area</t>
+          <t>Fort St John, British Columbia, Canada</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
@@ -811,201 +835,225 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lee Robert Gray </t>
+          <t>Jan Kyrstein</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Jan</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Gray</t>
+          <t>Kyrstein</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/lee-robert-gray-gradiosh-55b31a47</t>
+          <t>https://linkedin.com/in/jan-kyrstein-39007211</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Senior SHEQ Advisor</t>
+          <t xml:space="preserve">Construction Manager/Deputy Area Manager </t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Newcastle upon Tyne, England, United Kingdom</t>
+          <t>Fort St John, British Columbia, Canada</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>07872331053</t>
+          <t>+1 306-318-0214 , +1 604-563-5197</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>leergray3@hotmail.co.uk , lee.gray@mcaleer-rushe.co.uk</t>
+          <t>jan.kyrstein@pinnaclepellet.com , jan.kyrstein@bhpbilliton.com , kyrstein@technologist.com</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Eamonn Laverty</t>
+          <t>Dana Driver</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Eamonn</t>
+          <t>Dana</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Laverty</t>
+          <t>Driver</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/eamonn-laverty-mciob-9634b9b1</t>
+          <t>https://linkedin.com/in/dana-driver-crsp-9050584a</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Thornton Roofing</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Construction Operations Manager</t>
+          <t>District Safety Manager</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Ireland</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+          <t>Keeyask</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>DNC , +1 587-434-3086 , +1 403-280-2126</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>ddriver@flatironcorp.com</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Eoin Gormley</t>
+          <t>Mark Neis</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Eoin</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Gormley</t>
+          <t>Neis</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/eoin-gormley-10694a121</t>
+          <t>https://linkedin.com/in/mark-neis-27462812</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Project Director</t>
+          <t>Deputy Project Director</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>London Area, United Kingdom</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+          <t>Fort St John, British Columbia, Canada</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>+63 926 022 0867 , +63 942 908 8629</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>100267.2650@compuserve.com , mark.neis@cbi.com , mneis@flatironcorp.com</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Paddy Connolly</t>
+          <t>Joel Jacques</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Paddy</t>
+          <t>Joel</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Connolly</t>
+          <t>Jacques</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/paddy-connolly-3a4527102</t>
+          <t>https://linkedin.com/in/joel-jacques-p-eng-7072a655</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Coast Valley Contracting Ltd</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>President</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Belfast, Northern Ireland, United Kingdom</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+          <t>Squamish, British Columbia, Canada</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>+1 604-849-1017</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>joel.jacques@coastvalley.ca</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Daisy Butterworth</t>
+          <t>Fidel Velarde</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>Fidel</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Butterworth</t>
+          <t>Velarde</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/daisy-butterworth-14b437173</t>
+          <t>https://linkedin.com/in/fidel-velarde-054366164</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Assistant Project Manager</t>
+          <t>Quality Manager</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>London, England, United Kingdom</t>
+          <t>Richmond, British Columbia, Canada</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
@@ -1014,37 +1062,37 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sinead Gorman</t>
+          <t>Jenn Hirschman</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sinead</t>
+          <t>Jenn</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Gorman</t>
+          <t>Hirschman</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/sinéad-gorman-she-her-523b9a64</t>
+          <t>https://linkedin.com/in/jenn-hirschman-7b55a1167</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>SHEQ Officer</t>
+          <t>Health &amp; Safety Manager III</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Belfast, United Kingdom</t>
+          <t>British Columbia, Canada</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -1053,299 +1101,166 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Connor Graham</t>
+          <t>Pete Walton</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Connor</t>
+          <t>Pete</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Graham</t>
+          <t>Walton</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/connor-graham-50b2b241</t>
+          <t>https://linkedin.com/in/pete-walton</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Head of Buying</t>
+          <t>Canadian Division Safety Director</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Cookstown, N.Ireland</t>
+          <t>Alberta Construction Safety Association</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>+44 28 2565 0003</t>
+          <t>+1 970-290-8000 , +1 252-229-5369 , +1 303-579-7895 , +1 719-351-5126 , +1 224-578-1158 , +1 210-618-2993 , +1 956-467-6750</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>connor.graham@patton.co.uk , connor.graham@mcaleer-rushe.co.uk</t>
+          <t>plwalton@verizon.net , irmawalton@webtv.net</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Cathal Magee</t>
+          <t>Frank Mydlinski</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cathal</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Magee</t>
+          <t>Mydlinski</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/cathal-magee-a397ba8a</t>
+          <t>https://linkedin.com/in/frank-mydlinski-0566a184</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Health and Safety Officer</t>
+          <t>Senior Quality Manager</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>London, United Kingdom</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>+44 7835 631685</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>cathal.magee@mcaleer-rushe.co.uk , cathal.magee1@hotmail.co.uk</t>
-        </is>
-      </c>
+          <t>Chilliwack, British Columbia, Canada</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Bruno Antoniazzi</t>
+          <t>Husted Janet</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Bruno</t>
+          <t>Husted</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Antoniazzi</t>
+          <t>Janet</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/bruno-antoniazzi</t>
+          <t>https://linkedin.com/in/husted-janet-62b1b8116</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>M&amp;E</t>
+          <t>Health Safety Manager</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Cookstown</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>+55 21 98139-3298 , +55 92 98855-0059 , +55 92 98802-4114</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>bruno.antoniazzi@mcaleer-rushe.co.uk</t>
-        </is>
-      </c>
+          <t>Merritt, British Columbia, Canada</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nina Salandy </t>
+          <t>Hodge Garry</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Nina</t>
+          <t>Hodge</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Salandy</t>
+          <t>Garry</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/nina-salandy-bsc-hons-gradiosh-4675955a</t>
+          <t>https://linkedin.com/in/hodge-garry-a4a3a59b</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>McAleer &amp; Rushe</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Snr. SHEQ Advisor</t>
+          <t>PROJECT SAFETY MANAGER</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>London, England, United Kingdom</t>
+          <t>Greater Edmonton Metropolitan Area</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Peter Coyle</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Peter</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Coyle</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>https://linkedin.com/in/peter-coyle-854a8063</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>McAleer &amp; Rushe</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Senior Construction Manager</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Belfast, United Kingdom</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Orran Devine</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Orran</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Devine</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>https://linkedin.com/in/orran-devine-b2715b166</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>McAleer &amp; Rushe</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Project Manager</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Cookstown, Northern Ireland, United Kingdom</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Niamh Heneghan</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Niamh</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Heneghan</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>https://linkedin.com/in/niamh-heneghan-a98527197</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>McAleer &amp; Rushe</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Health and safety administrator</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Wembley, England, United Kingdom</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
2023-11-21 02:47:56 - phone regex
</commit_message>
<xml_diff>
--- a/server/output/output.xlsx
+++ b/server/output/output.xlsx
@@ -461,22 +461,22 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Job</t>
+          <t>Title</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Country</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Phones</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Emails</t>
+          <t>Email</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Calgary, Alberta, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>paul.newman@snclavalin.com , paul@pave-it.com , pnewman@bellsouth.net</t>
+          <t>Email Invalid</t>
         </is>
       </c>
     </row>
@@ -560,11 +560,15 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Calgary, Alberta, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nlynchehaun@flatironcorp.com</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -646,11 +650,15 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>British Columbia, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Email Invalid</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -685,7 +693,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Richmond, BC, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -732,7 +740,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">USA and Canada </t>
+          <t>United States</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -779,7 +787,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>British Columbia, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -789,7 +797,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>mike.meacher@lafarge-na.com , mmeacher@fwsgroup.com , mmeacher@flatironcorp.com</t>
+          <t>mmeacher@flatironcorp.com</t>
         </is>
       </c>
     </row>
@@ -826,11 +834,15 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Fort St John, British Columbia, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Email Invalid</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -865,7 +877,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Fort St John, British Columbia, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -875,7 +887,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>jan.kyrstein@pinnaclepellet.com , jan.kyrstein@bhpbilliton.com , kyrstein@technologist.com</t>
+          <t>Email Invalid</t>
         </is>
       </c>
     </row>
@@ -959,7 +971,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Fort St John, British Columbia, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -969,7 +981,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>100267.2650@compuserve.com , mark.neis@cbi.com , mneis@flatironcorp.com</t>
+          <t>mneis@flatironcorp.com</t>
         </is>
       </c>
     </row>
@@ -1006,7 +1018,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Squamish, British Columbia, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1053,11 +1065,15 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Richmond, British Columbia, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>fvelarde@flatironcorp.com</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1092,11 +1108,15 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>British Columbia, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Email Invalid</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1141,7 +1161,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>plwalton@verizon.net , irmawalton@webtv.net</t>
+          <t>Email Invalid</t>
         </is>
       </c>
     </row>
@@ -1178,11 +1198,15 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Chilliwack, British Columbia, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Email Invalid</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1217,11 +1241,15 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Merritt, British Columbia, Canada</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Email Invalid</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1260,7 +1288,11 @@
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Email Invalid</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
2023-11-21 22:35:47 - algo prev
</commit_message>
<xml_diff>
--- a/server/output/output.xlsx
+++ b/server/output/output.xlsx
@@ -566,7 +566,7 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>nlynchehaun@flatironcorp.com</t>
+          <t>Email Invalid</t>
         </is>
       </c>
     </row>
@@ -1114,7 +1114,7 @@
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Email Invalid</t>
+          <t>jhirschman@flatironcorp.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
2023-11-24 02:48:29 - zerobounce changes
</commit_message>
<xml_diff>
--- a/server/output/output.xlsx
+++ b/server/output/output.xlsx
@@ -521,11 +521,7 @@
           <t>+1 403-701-8000 , +1 403-589-9088 , +1 403-620-7239 , +1 410-340-7346 , +1 418-868-2428 , +1 403-640-3521</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Email Invalid</t>
-        </is>
-      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -566,7 +562,7 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Email Invalid</t>
+          <t>Email not guessed from zerobounce</t>
         </is>
       </c>
     </row>
@@ -656,7 +652,7 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Email Invalid</t>
+          <t>Email not guessed from zerobounce</t>
         </is>
       </c>
     </row>
@@ -838,11 +834,7 @@
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Email Invalid</t>
-        </is>
-      </c>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -887,7 +879,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Email Invalid</t>
+          <t>Email not guessed from zerobounce</t>
         </is>
       </c>
     </row>
@@ -1071,7 +1063,7 @@
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>fvelarde@flatironcorp.com</t>
+          <t>Email not guessed from zerobounce</t>
         </is>
       </c>
     </row>
@@ -1114,7 +1106,7 @@
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>jhirschman@flatironcorp.com</t>
+          <t>Email not guessed from zerobounce</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1153,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Email Invalid</t>
+          <t>Email not guessed from zerobounce</t>
         </is>
       </c>
     </row>
@@ -1204,7 +1196,7 @@
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Email Invalid</t>
+          <t>Email not guessed from zerobounce</t>
         </is>
       </c>
     </row>
@@ -1247,7 +1239,7 @@
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Email Invalid</t>
+          <t>jhusted@flatironcorp.com</t>
         </is>
       </c>
     </row>
@@ -1290,7 +1282,7 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Email Invalid</t>
+          <t>Email not guessed from zerobounce</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
2023-12-04 03:44:54 - added bull
</commit_message>
<xml_diff>
--- a/server/output/output.xlsx
+++ b/server/output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,32 +451,27 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Linkedin</t>
+          <t>Company</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Company</t>
+          <t>Job</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
+          <t>Phones</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Phone</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
+          <t>Emails</t>
         </is>
       </c>
     </row>
@@ -498,30 +493,25 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/paul-newman-00a9a830</t>
+          <t>Bow Transit Connectors</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Bow Transit Connectors</t>
+          <t>Construction Manager</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Construction Manager</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
           <t>+1 403-701-8000 , +1 403-589-9088 , +1 403-620-7239 , +1 410-340-7346 , +1 418-868-2428 , +1 403-640-3521</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -541,26 +531,21 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/neil-lynchehaun-23031ba4</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>Vice President, Special Projects</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Vice President, Special Projects</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Email not guessed from zerobounce</t>
         </is>
@@ -584,30 +569,25 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/ken-tanner-9899939</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>Vice President Operations</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Vice President Operations</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>+1 604-798-8491</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
-        <is>
-          <t>+1 604-798-8491</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
         <is>
           <t>ktanner@flatironcorp.com</t>
         </is>
@@ -631,26 +611,21 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/octavio-flores-37b566a7</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>Area Operations Manager</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Area Operations Manager</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
         <is>
           <t>Email not guessed from zerobounce</t>
         </is>
@@ -674,30 +649,25 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/jarredgumbleton</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>Project Manager</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>+1 250-272-6645</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
-        <is>
-          <t>+1 250-272-6645</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
         <is>
           <t>jgumbleton@flatironcorp.com</t>
         </is>
@@ -721,30 +691,25 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/alicialopezcrespo</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>VP, Innovation &amp; Design</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>VP, Innovation &amp; Design</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>DNC , DNC , +1 719-994-0855 , +1 720-232-3886 , DNC</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
-        <is>
-          <t>DNC , DNC , +1 719-994-0855 , +1 720-232-3886 , DNC</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
         <is>
           <t>acrespo@flatironcorp.com</t>
         </is>
@@ -768,30 +733,25 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/mike-meacher-031ba619</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>Quality Manager</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Quality Manager</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>+1 604-363-4558</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
-        <is>
-          <t>+1 604-363-4558</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
         <is>
           <t>mmeacher@flatironcorp.com</t>
         </is>
@@ -815,26 +775,21 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/donald-dow-7518ab192</t>
+          <t>AFDE Partnership</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>AFDE Partnership</t>
+          <t>Safety Manager</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Safety Manager</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -854,30 +809,25 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/jan-kyrstein-39007211</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t xml:space="preserve">Construction Manager/Deputy Area Manager </t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Construction Manager/Deputy Area Manager </t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>+1 306-318-0214 , +1 604-563-5197</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
-        <is>
-          <t>+1 306-318-0214 , +1 604-563-5197</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
         <is>
           <t>Email not guessed from zerobounce</t>
         </is>
@@ -901,30 +851,25 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/dana-driver-crsp-9050584a</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>District Safety Manager</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>District Safety Manager</t>
+          <t>Keeyask</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Keeyask</t>
+          <t>DNC , +1 587-434-3086 , +1 403-280-2126</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
-        <is>
-          <t>DNC , +1 587-434-3086 , +1 403-280-2126</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
         <is>
           <t>ddriver@flatironcorp.com</t>
         </is>
@@ -948,30 +893,25 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/mark-neis-27462812</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>Deputy Project Director</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Deputy Project Director</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>+63 926 022 0867 , +63 942 908 8629</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
-        <is>
-          <t>+63 926 022 0867 , +63 942 908 8629</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
         <is>
           <t>mneis@flatironcorp.com</t>
         </is>
@@ -995,30 +935,25 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/joel-jacques-p-eng-7072a655</t>
+          <t>Coast Valley Contracting Ltd</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Coast Valley Contracting Ltd</t>
+          <t>President</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>President</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>+1 604-849-1017</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
-        <is>
-          <t>+1 604-849-1017</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
         <is>
           <t>joel.jacques@coastvalley.ca</t>
         </is>
@@ -1042,26 +977,21 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/fidel-velarde-054366164</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>Quality Manager</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Quality Manager</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
         <is>
           <t>Email not guessed from zerobounce</t>
         </is>
@@ -1085,26 +1015,21 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/jenn-hirschman-7b55a1167</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>Health &amp; Safety Manager III</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Health &amp; Safety Manager III</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
         <is>
           <t>Email not guessed from zerobounce</t>
         </is>
@@ -1128,30 +1053,25 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/pete-walton</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>Canadian Division Safety Director</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Canadian Division Safety Director</t>
+          <t>Alberta Construction Safety Association</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Alberta Construction Safety Association</t>
+          <t>+1 970-290-8000 , +1 252-229-5369 , +1 303-579-7895 , +1 719-351-5126 , +1 224-578-1158 , +1 210-618-2993 , +1 956-467-6750</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
-        <is>
-          <t>+1 970-290-8000 , +1 252-229-5369 , +1 303-579-7895 , +1 719-351-5126 , +1 224-578-1158 , +1 210-618-2993 , +1 956-467-6750</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
         <is>
           <t>Email not guessed from zerobounce</t>
         </is>
@@ -1175,26 +1095,21 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/frank-mydlinski-0566a184</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>Senior Quality Manager</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Senior Quality Manager</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr">
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
         <is>
           <t>Email not guessed from zerobounce</t>
         </is>
@@ -1218,26 +1133,21 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/husted-janet-62b1b8116</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>Health Safety Manager</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Health Safety Manager</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr">
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
         <is>
           <t>jhusted@flatironcorp.com</t>
         </is>
@@ -1261,26 +1171,21 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/hodge-garry-a4a3a59b</t>
+          <t>Flatiron Construction</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Flatiron Construction</t>
+          <t>PROJECT SAFETY MANAGER</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>PROJECT SAFETY MANAGER</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
           <t>Greater Edmonton Metropolitan Area</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr">
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
         <is>
           <t>Email not guessed from zerobounce</t>
         </is>

</xml_diff>